<commit_message>
adding data to the data folder
</commit_message>
<xml_diff>
--- a/fa23-team/src/Unemployment_2020-2023.xlsx
+++ b/fa23-team/src/Unemployment_2020-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leeseunghee/Documents/MSDSBU/FALL2023/DS701/ds-bch-vaccine-equity/fa23-team/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E218E5-9C76-4646-9CF4-2D4FE4E50912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FF372A-1884-374D-AFF9-47DBC6494D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17420" yWindow="-21760" windowWidth="24420" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Unemployment_2020-202" sheetId="1" r:id="rId1"/>
@@ -1417,9 +1417,7 @@
   </sheetPr>
   <dimension ref="A1:H240"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>